<commit_message>
Add file & fixed bugs --- - Add file load transaction by address
</commit_message>
<xml_diff>
--- a/data/List of well-known Names used to identify accounts.xlsx
+++ b/data/List of well-known Names used to identify accounts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7592,7 +7592,7 @@
   <dimension ref="A1:H872"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G875" sqref="G875"/>
+      <selection activeCell="C876" sqref="C876"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>